<commit_message>
Finalize prosumer outputs under service level constraint
</commit_message>
<xml_diff>
--- a/Outputs/4. Prosumer percentage constrained/Grid Search/Evaluation Metrics.xlsx
+++ b/Outputs/4. Prosumer percentage constrained/Grid Search/Evaluation Metrics.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/Github/microgrid_MP/Outputs/4. Prosumer percentage constrained/Grid Search/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mailaub-my.sharepoint.com/personal/mo10_aub_edu_lb/Documents/3-Research/Elsa/Model 1/ud_penalty/Outputs/4. Prosumer percentage constrained/Grid Search/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="11_085DD8C79750160F6235547658FFCEF98A1D84F9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6059DD58-2E52-4F8B-83F4-321E08CF5B2C}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_085D49E79048940F6235547658EA567DBF2184D5" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4D1F21CC-A38D-4578-9BE7-D24AF5E37191}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2620" yWindow="2620" windowWidth="14400" windowHeight="8250" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -59,6 +72,7 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -406,17 +420,10 @@
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.54296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.453125" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
@@ -446,13 +453,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.09</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C2">
         <v>0.4</v>
       </c>
       <c r="D2">
-        <v>6.5194514888494244E-3</v>
+        <v>6.5194514888494903E-3</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -469,19 +476,19 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>7.0000000000000007E-2</v>
+        <v>0.17</v>
       </c>
       <c r="C3">
-        <v>0.38</v>
+        <v>0.39</v>
       </c>
       <c r="D3">
-        <v>1.716658014495755E-2</v>
+        <v>1.7166580144957491E-2</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
       <c r="F3">
-        <v>8838088.8960245438</v>
+        <v>8840178.3152753748</v>
       </c>
       <c r="G3">
         <v>0</v>
@@ -521,16 +528,16 @@
         <v>0.32</v>
       </c>
       <c r="D5">
-        <v>1.933429637454015E-2</v>
+        <v>1.9334296374540139E-2</v>
       </c>
       <c r="E5">
-        <v>6.2840615108861075E-2</v>
+        <v>6.2840615108861048E-2</v>
       </c>
       <c r="F5">
-        <v>9146002.7733741365</v>
+        <v>9146002.7733741403</v>
       </c>
       <c r="G5">
-        <v>3.6962696997926377E-2</v>
+        <v>3.6962696997926363E-2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
@@ -544,16 +551,16 @@
         <v>0.28000000000000003</v>
       </c>
       <c r="D6">
-        <v>1.7536085010108719E-2</v>
+        <v>1.7536085010108709E-2</v>
       </c>
       <c r="E6">
-        <v>1.396759646333974E-2</v>
+        <v>1.3967596463339759E-2</v>
       </c>
       <c r="F6">
-        <v>9143534.0149630625</v>
+        <v>9143534.0149630606</v>
       </c>
       <c r="G6">
-        <v>8.2157062748250357E-3</v>
+        <v>8.2157062748250461E-3</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
@@ -570,13 +577,13 @@
         <v>1.550705288481463E-2</v>
       </c>
       <c r="E7">
-        <v>0.1092076982182444</v>
+        <v>0.1113969968370139</v>
       </c>
       <c r="F7">
-        <v>8928223.8400191143</v>
+        <v>8927469.1720317546</v>
       </c>
       <c r="G7">
-        <v>6.423570253233811E-2</v>
+        <v>6.552344265619546E-2</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
@@ -584,22 +591,22 @@
         <v>75</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>0.04</v>
       </c>
       <c r="C8">
-        <v>0.25</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="D8">
         <v>1.393761746878331E-2</v>
       </c>
       <c r="E8">
-        <v>0.30594979084808732</v>
+        <v>0.24690013833237789</v>
       </c>
       <c r="F8">
-        <v>8349374.2108064964</v>
+        <v>8397441.337237617</v>
       </c>
       <c r="G8">
-        <v>0.17995892300077379</v>
+        <v>0.1452260609816807</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
@@ -607,22 +614,22 @@
         <v>90</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="C9">
-        <v>0.24</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="D9">
-        <v>1.8029877187196688E-2</v>
+        <v>1.8029877187196681E-2</v>
       </c>
       <c r="E9">
-        <v>0.45309422669325577</v>
+        <v>0.38828426439893238</v>
       </c>
       <c r="F9">
-        <v>7598902.7724572076</v>
+        <v>7653183.6090507964</v>
       </c>
       <c r="G9">
-        <v>0.26650892235475609</v>
+        <v>0.22838786013118931</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
@@ -630,22 +637,22 @@
         <v>100</v>
       </c>
       <c r="B10">
-        <v>0.06</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C10">
-        <v>0.28999999999999998</v>
+        <v>0.3</v>
       </c>
       <c r="D10">
-        <v>2.4472325223299639E-2</v>
+        <v>1.386146741153913E-2</v>
       </c>
       <c r="E10">
-        <v>0.49346950508287418</v>
+        <v>0.47410653732625269</v>
       </c>
       <c r="F10">
-        <v>7000612.9452658705</v>
+        <v>7089451.9449234158</v>
       </c>
       <c r="G10">
-        <v>0.29025756292323401</v>
+        <v>0.27886831237358911</v>
       </c>
     </row>
   </sheetData>

</xml_diff>